<commit_message>
bat files added and notification handled
</commit_message>
<xml_diff>
--- a/TestData/hack_excel.xlsx
+++ b/TestData/hack_excel.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="34">
   <si>
     <t>Plans</t>
   </si>
@@ -122,6 +122,24 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>Royal Sundaram</t>
+  </si>
+  <si>
+    <t>₹874</t>
+  </si>
+  <si>
+    <t>Travel Shield Single Trip</t>
+  </si>
+  <si>
+    <t>₹874GST included</t>
+  </si>
+  <si>
+    <t>₹1,220GST included</t>
+  </si>
+  <si>
+    <t>₹1,333GST included</t>
   </si>
 </sst>
 </file>
@@ -496,26 +514,26 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>